<commit_message>
RegistrarAdmin y Correccion HU
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACION/1.3 Historias de Usuario/3. Plantilla_Matriz_Marco_Trabajo_HU_V1.2.xlsx
+++ b/PREGAME/1. ELICITACION/1.3 Historias de Usuario/3. Plantilla_Matriz_Marco_Trabajo_HU_V1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semestres\Semestre 2022-2023\Analisis y Diseño de SW\Repositorio\8311_G4_ADSW\PREGAME\1. ELICITACION\1.3 Historias de Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19EB932-E1C2-45D7-A4E6-B50FDB02E392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31D424C-2B19-4E70-BEBD-1BAF30B7D6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,6 +886,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -894,19 +900,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -914,6 +912,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1811,8 +1811,8 @@
   </sheetPr>
   <dimension ref="B1:O1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2009,7 +2009,7 @@
         <v>84</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="G8" s="37" t="s">
         <v>85</v>
@@ -8222,15 +8222,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="16"/>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="69"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="69"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
@@ -8245,17 +8245,17 @@
         <v>38</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="70" t="str">
+      <c r="E10" s="68" t="str">
         <f>VLOOKUP('Historia de Usuario'!C10,'Formato descripción HU'!B6:O12,5,0)</f>
         <v>Administrador</v>
       </c>
-      <c r="F10" s="69"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="70" t="str">
+      <c r="H10" s="68" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,11,0)</f>
         <v>Terminado</v>
       </c>
-      <c r="I10" s="69"/>
+      <c r="I10" s="67"/>
       <c r="J10" s="20"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -8287,15 +8287,15 @@
         <v>71</v>
       </c>
       <c r="D12" s="19"/>
-      <c r="E12" s="68" t="s">
+      <c r="E12" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="69"/>
+      <c r="F12" s="67"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="69"/>
+      <c r="I12" s="67"/>
       <c r="J12" s="20"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
@@ -8311,17 +8311,17 @@
         <v>5</v>
       </c>
       <c r="D13" s="19"/>
-      <c r="E13" s="70" t="str">
+      <c r="E13" s="68" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,10,0)</f>
         <v>Alta</v>
       </c>
-      <c r="F13" s="69"/>
+      <c r="F13" s="67"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="70" t="str">
+      <c r="H13" s="68" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,7,0)</f>
         <v>Freddy Páez</v>
       </c>
-      <c r="I13" s="69"/>
+      <c r="I13" s="67"/>
       <c r="J13" s="20"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
@@ -8356,7 +8356,7 @@
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,3,0)</f>
         <v>Permite el inicio de sesión al administrador</v>
       </c>
-      <c r="E15" s="60"/>
+      <c r="E15" s="54"/>
       <c r="F15" s="17"/>
       <c r="G15" s="41" t="s">
         <v>74</v>
@@ -8365,8 +8365,8 @@
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,4,0)</f>
         <v>Iniciar sesión como administrador</v>
       </c>
-      <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="54"/>
       <c r="K15" s="17"/>
       <c r="L15" s="41" t="s">
         <v>75</v>
@@ -8382,13 +8382,13 @@
     <row r="16" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="31"/>
       <c r="C16" s="42"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="62"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
       <c r="F16" s="17"/>
       <c r="G16" s="42"/>
-      <c r="H16" s="61"/>
+      <c r="H16" s="64"/>
       <c r="I16" s="40"/>
-      <c r="J16" s="62"/>
+      <c r="J16" s="65"/>
       <c r="K16" s="17"/>
       <c r="L16" s="42"/>
       <c r="M16" s="47"/>
@@ -8399,13 +8399,13 @@
     <row r="17" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="31"/>
       <c r="C17" s="43"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="65"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="17"/>
       <c r="G17" s="43"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="65"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="56"/>
       <c r="K17" s="17"/>
       <c r="L17" s="43"/>
       <c r="M17" s="50"/>
@@ -8432,41 +8432,41 @@
     </row>
     <row r="19" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="31"/>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="53" t="str">
+      <c r="D19" s="54"/>
+      <c r="E19" s="57" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,14,0)</f>
         <v>Iniciar sesión como administrador</v>
       </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="55"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="59"/>
       <c r="P19" s="32"/>
     </row>
     <row r="20" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="31"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="58"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="62"/>
       <c r="P20" s="32"/>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8488,10 +8488,10 @@
     </row>
     <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="31"/>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="60"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="44" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,12,0)</f>
         <v>Pruebas Unitarias que permitan validar que los datos ingresados sean los correctos.</v>
@@ -8500,10 +8500,10 @@
       <c r="G22" s="45"/>
       <c r="H22" s="46"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="66" t="s">
+      <c r="J22" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="60"/>
+      <c r="K22" s="54"/>
       <c r="L22" s="44">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O12,13,0)</f>
         <v>0</v>
@@ -8515,15 +8515,15 @@
     </row>
     <row r="23" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="31"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="62"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="47"/>
       <c r="F23" s="48"/>
       <c r="G23" s="48"/>
       <c r="H23" s="49"/>
       <c r="I23" s="17"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="62"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="65"/>
       <c r="L23" s="47"/>
       <c r="M23" s="48"/>
       <c r="N23" s="48"/>
@@ -8532,15 +8532,15 @@
     </row>
     <row r="24" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="31"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="65"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="50"/>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
       <c r="H24" s="52"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="65"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="56"/>
       <c r="L24" s="50"/>
       <c r="M24" s="51"/>
       <c r="N24" s="51"/>
@@ -8604,15 +8604,15 @@
         <v>1</v>
       </c>
       <c r="D30" s="16"/>
-      <c r="E30" s="68" t="s">
+      <c r="E30" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="69"/>
+      <c r="F30" s="67"/>
       <c r="G30" s="16"/>
-      <c r="H30" s="68" t="s">
+      <c r="H30" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="69"/>
+      <c r="I30" s="67"/>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
       <c r="L30" s="17"/>
@@ -8627,10 +8627,10 @@
         <v>20</v>
       </c>
       <c r="D31" s="19"/>
-      <c r="E31" s="70" t="s">
+      <c r="E31" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="69"/>
+      <c r="F31" s="67"/>
       <c r="G31" s="20"/>
       <c r="H31" s="73" t="s">
         <v>78</v>
@@ -8667,15 +8667,15 @@
         <v>71</v>
       </c>
       <c r="D33" s="19"/>
-      <c r="E33" s="68" t="s">
+      <c r="E33" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="69"/>
+      <c r="F33" s="67"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="68" t="s">
+      <c r="H33" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="I33" s="69"/>
+      <c r="I33" s="67"/>
       <c r="J33" s="20"/>
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
@@ -8691,15 +8691,15 @@
         <v>5</v>
       </c>
       <c r="D34" s="19"/>
-      <c r="E34" s="70" t="s">
+      <c r="E34" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="F34" s="69"/>
+      <c r="F34" s="67"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="70" t="s">
+      <c r="H34" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="69"/>
+      <c r="I34" s="67"/>
       <c r="J34" s="20"/>
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
@@ -8734,7 +8734,7 @@
         <f>VLOOKUP(C31,'Formato descripción HU'!B6:O7,3,0)</f>
         <v>Eliminar productos del catalogo</v>
       </c>
-      <c r="E36" s="60"/>
+      <c r="E36" s="54"/>
       <c r="F36" s="17"/>
       <c r="G36" s="41" t="s">
         <v>74</v>
@@ -8743,8 +8743,8 @@
         <f>VLOOKUP(C31,'Formato descripción HU'!B6:O7,4,0)</f>
         <v>Tener registrados unicamente protuctos en stock</v>
       </c>
-      <c r="I36" s="59"/>
-      <c r="J36" s="60"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="54"/>
       <c r="K36" s="17"/>
       <c r="L36" s="41" t="s">
         <v>75</v>
@@ -8760,13 +8760,13 @@
     <row r="37" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="31"/>
       <c r="C37" s="42"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="62"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="65"/>
       <c r="F37" s="17"/>
       <c r="G37" s="42"/>
-      <c r="H37" s="61"/>
+      <c r="H37" s="64"/>
       <c r="I37" s="40"/>
-      <c r="J37" s="62"/>
+      <c r="J37" s="65"/>
       <c r="K37" s="17"/>
       <c r="L37" s="42"/>
       <c r="M37" s="47"/>
@@ -8777,13 +8777,13 @@
     <row r="38" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="31"/>
       <c r="C38" s="43"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="65"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="56"/>
       <c r="F38" s="17"/>
       <c r="G38" s="43"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="64"/>
-      <c r="J38" s="65"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="56"/>
       <c r="K38" s="17"/>
       <c r="L38" s="43"/>
       <c r="M38" s="50"/>
@@ -8810,40 +8810,40 @@
     </row>
     <row r="40" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="31"/>
-      <c r="C40" s="67" t="s">
+      <c r="C40" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="53" t="s">
+      <c r="D40" s="54"/>
+      <c r="E40" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="54"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="54"/>
-      <c r="O40" s="55"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="59"/>
       <c r="P40" s="32"/>
     </row>
     <row r="41" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="31"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="57"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="57"/>
-      <c r="M41" s="57"/>
-      <c r="N41" s="57"/>
-      <c r="O41" s="58"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+      <c r="L41" s="61"/>
+      <c r="M41" s="61"/>
+      <c r="N41" s="61"/>
+      <c r="O41" s="62"/>
       <c r="P41" s="32"/>
     </row>
     <row r="42" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8865,10 +8865,10 @@
     </row>
     <row r="43" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="31"/>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="60"/>
+      <c r="D43" s="54"/>
       <c r="E43" s="44" t="str">
         <f>VLOOKUP(C31,'Formato descripción HU'!B6:O7,12,0)</f>
         <v>Pruebas Unitarias que verifiquen que el producto se eliminó del catálogo (mensaje eliminado correctamente)</v>
@@ -8877,10 +8877,10 @@
       <c r="G43" s="45"/>
       <c r="H43" s="46"/>
       <c r="I43" s="17"/>
-      <c r="J43" s="66" t="s">
+      <c r="J43" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="K43" s="60"/>
+      <c r="K43" s="54"/>
       <c r="L43" s="44" t="str">
         <f>VLOOKUP(C31,'Formato descripción HU'!B6:O7,13,0)</f>
         <v>Para la eliminación de un producto este primero debe estar registrado dentro del catálogo</v>
@@ -8892,15 +8892,15 @@
     </row>
     <row r="44" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="31"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="62"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="65"/>
       <c r="E44" s="47"/>
       <c r="F44" s="48"/>
       <c r="G44" s="48"/>
       <c r="H44" s="49"/>
       <c r="I44" s="17"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="62"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="65"/>
       <c r="L44" s="47"/>
       <c r="M44" s="48"/>
       <c r="N44" s="48"/>
@@ -8909,15 +8909,15 @@
     </row>
     <row r="45" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="65"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="50"/>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
       <c r="H45" s="52"/>
       <c r="I45" s="17"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="65"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="56"/>
       <c r="L45" s="50"/>
       <c r="M45" s="51"/>
       <c r="N45" s="51"/>
@@ -8999,15 +8999,15 @@
         <v>1</v>
       </c>
       <c r="D51" s="16"/>
-      <c r="E51" s="68" t="s">
+      <c r="E51" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F51" s="69"/>
+      <c r="F51" s="67"/>
       <c r="G51" s="16"/>
-      <c r="H51" s="68" t="s">
+      <c r="H51" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="69"/>
+      <c r="I51" s="67"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
@@ -9022,11 +9022,11 @@
         <v>29</v>
       </c>
       <c r="D52" s="19"/>
-      <c r="E52" s="70" t="e">
+      <c r="E52" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C52,'Formato descripción HU'!#REF!,5,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="F52" s="69"/>
+      <c r="F52" s="67"/>
       <c r="G52" s="20"/>
       <c r="H52" s="73" t="e">
         <f>VLOOKUP('Historia de Usuario'!C52,'Formato descripción HU'!#REF!,11,0)</f>
@@ -9064,15 +9064,15 @@
         <v>71</v>
       </c>
       <c r="D54" s="19"/>
-      <c r="E54" s="68" t="s">
+      <c r="E54" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="F54" s="69"/>
+      <c r="F54" s="67"/>
       <c r="G54" s="20"/>
-      <c r="H54" s="68" t="s">
+      <c r="H54" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="I54" s="69"/>
+      <c r="I54" s="67"/>
       <c r="J54" s="20"/>
       <c r="K54" s="21"/>
       <c r="L54" s="21"/>
@@ -9088,17 +9088,17 @@
         <v>#N/A</v>
       </c>
       <c r="D55" s="19"/>
-      <c r="E55" s="70" t="e">
+      <c r="E55" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C52,'Formato descripción HU'!#REF!,10,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="F55" s="69"/>
+      <c r="F55" s="67"/>
       <c r="G55" s="20"/>
-      <c r="H55" s="70" t="e">
+      <c r="H55" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C52,'Formato descripción HU'!#REF!,7,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="I55" s="69"/>
+      <c r="I55" s="67"/>
       <c r="J55" s="20"/>
       <c r="K55" s="21"/>
       <c r="L55" s="21"/>
@@ -9133,7 +9133,7 @@
         <f>VLOOKUP(C52,'Formato descripción HU'!#REF!,3,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="E57" s="60"/>
+      <c r="E57" s="54"/>
       <c r="F57" s="17"/>
       <c r="G57" s="41" t="s">
         <v>74</v>
@@ -9142,8 +9142,8 @@
         <f>VLOOKUP(C52,'Formato descripción HU'!#REF!,4,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="I57" s="59"/>
-      <c r="J57" s="60"/>
+      <c r="I57" s="69"/>
+      <c r="J57" s="54"/>
       <c r="K57" s="17"/>
       <c r="L57" s="41" t="s">
         <v>75</v>
@@ -9159,13 +9159,13 @@
     <row r="58" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="31"/>
       <c r="C58" s="42"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="62"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="65"/>
       <c r="F58" s="17"/>
       <c r="G58" s="42"/>
-      <c r="H58" s="61"/>
+      <c r="H58" s="64"/>
       <c r="I58" s="40"/>
-      <c r="J58" s="62"/>
+      <c r="J58" s="65"/>
       <c r="K58" s="17"/>
       <c r="L58" s="42"/>
       <c r="M58" s="47"/>
@@ -9176,13 +9176,13 @@
     <row r="59" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="31"/>
       <c r="C59" s="43"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="65"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="56"/>
       <c r="F59" s="17"/>
       <c r="G59" s="43"/>
-      <c r="H59" s="63"/>
-      <c r="I59" s="64"/>
-      <c r="J59" s="65"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="70"/>
+      <c r="J59" s="56"/>
       <c r="K59" s="17"/>
       <c r="L59" s="43"/>
       <c r="M59" s="50"/>
@@ -9209,41 +9209,41 @@
     </row>
     <row r="61" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="31"/>
-      <c r="C61" s="67" t="s">
+      <c r="C61" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="D61" s="60"/>
-      <c r="E61" s="53" t="e">
+      <c r="D61" s="54"/>
+      <c r="E61" s="57" t="e">
         <f>VLOOKUP('Historia de Usuario'!C52,'Formato descripción HU'!#REF!,14,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="F61" s="54"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="54"/>
-      <c r="J61" s="54"/>
-      <c r="K61" s="54"/>
-      <c r="L61" s="54"/>
-      <c r="M61" s="54"/>
-      <c r="N61" s="54"/>
-      <c r="O61" s="55"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="58"/>
+      <c r="J61" s="58"/>
+      <c r="K61" s="58"/>
+      <c r="L61" s="58"/>
+      <c r="M61" s="58"/>
+      <c r="N61" s="58"/>
+      <c r="O61" s="59"/>
       <c r="P61" s="32"/>
     </row>
     <row r="62" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="31"/>
-      <c r="C62" s="63"/>
-      <c r="D62" s="65"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="57"/>
-      <c r="M62" s="57"/>
-      <c r="N62" s="57"/>
-      <c r="O62" s="58"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="60"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="61"/>
+      <c r="K62" s="61"/>
+      <c r="L62" s="61"/>
+      <c r="M62" s="61"/>
+      <c r="N62" s="61"/>
+      <c r="O62" s="62"/>
       <c r="P62" s="32"/>
     </row>
     <row r="63" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9265,10 +9265,10 @@
     </row>
     <row r="64" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="31"/>
-      <c r="C64" s="66" t="s">
+      <c r="C64" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="60"/>
+      <c r="D64" s="54"/>
       <c r="E64" s="44" t="e">
         <f>VLOOKUP(C52,'Formato descripción HU'!#REF!,12,0)</f>
         <v>#REF!</v>
@@ -9277,10 +9277,10 @@
       <c r="G64" s="45"/>
       <c r="H64" s="46"/>
       <c r="I64" s="17"/>
-      <c r="J64" s="66" t="s">
+      <c r="J64" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="K64" s="60"/>
+      <c r="K64" s="54"/>
       <c r="L64" s="44" t="e">
         <f>VLOOKUP(C52,'Formato descripción HU'!#REF!,13,0)</f>
         <v>#REF!</v>
@@ -9292,15 +9292,15 @@
     </row>
     <row r="65" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="31"/>
-      <c r="C65" s="61"/>
-      <c r="D65" s="62"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="65"/>
       <c r="E65" s="47"/>
       <c r="F65" s="48"/>
       <c r="G65" s="48"/>
       <c r="H65" s="49"/>
       <c r="I65" s="17"/>
-      <c r="J65" s="61"/>
-      <c r="K65" s="62"/>
+      <c r="J65" s="64"/>
+      <c r="K65" s="65"/>
       <c r="L65" s="47"/>
       <c r="M65" s="48"/>
       <c r="N65" s="48"/>
@@ -9309,15 +9309,15 @@
     </row>
     <row r="66" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="31"/>
-      <c r="C66" s="63"/>
-      <c r="D66" s="65"/>
+      <c r="C66" s="55"/>
+      <c r="D66" s="56"/>
       <c r="E66" s="50"/>
       <c r="F66" s="51"/>
       <c r="G66" s="51"/>
       <c r="H66" s="52"/>
       <c r="I66" s="17"/>
-      <c r="J66" s="63"/>
-      <c r="K66" s="65"/>
+      <c r="J66" s="55"/>
+      <c r="K66" s="56"/>
       <c r="L66" s="50"/>
       <c r="M66" s="51"/>
       <c r="N66" s="51"/>
@@ -9416,15 +9416,15 @@
         <v>1</v>
       </c>
       <c r="D73" s="16"/>
-      <c r="E73" s="68" t="s">
+      <c r="E73" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F73" s="69"/>
+      <c r="F73" s="67"/>
       <c r="G73" s="16"/>
-      <c r="H73" s="68" t="s">
+      <c r="H73" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I73" s="69"/>
+      <c r="I73" s="67"/>
       <c r="J73" s="17"/>
       <c r="K73" s="17"/>
       <c r="L73" s="17"/>
@@ -9439,11 +9439,11 @@
         <v>29</v>
       </c>
       <c r="D74" s="19"/>
-      <c r="E74" s="70" t="e">
+      <c r="E74" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C74,'Formato descripción HU'!B29:O29,5,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F74" s="69"/>
+      <c r="F74" s="67"/>
       <c r="G74" s="20"/>
       <c r="H74" s="73" t="e">
         <f>VLOOKUP('Historia de Usuario'!C74,'Formato descripción HU'!B29:O29,11,0)</f>
@@ -9481,15 +9481,15 @@
         <v>71</v>
       </c>
       <c r="D76" s="19"/>
-      <c r="E76" s="68" t="s">
+      <c r="E76" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="F76" s="69"/>
+      <c r="F76" s="67"/>
       <c r="G76" s="20"/>
-      <c r="H76" s="68" t="s">
+      <c r="H76" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="I76" s="69"/>
+      <c r="I76" s="67"/>
       <c r="J76" s="20"/>
       <c r="K76" s="21"/>
       <c r="L76" s="21"/>
@@ -9505,17 +9505,17 @@
         <v>#N/A</v>
       </c>
       <c r="D77" s="19"/>
-      <c r="E77" s="70" t="e">
+      <c r="E77" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C74,'Formato descripción HU'!B29:O29,10,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F77" s="69"/>
+      <c r="F77" s="67"/>
       <c r="G77" s="20"/>
-      <c r="H77" s="70" t="e">
+      <c r="H77" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C74,'Formato descripción HU'!B29:O29,7,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I77" s="69"/>
+      <c r="I77" s="67"/>
       <c r="J77" s="20"/>
       <c r="K77" s="21"/>
       <c r="L77" s="21"/>
@@ -9550,7 +9550,7 @@
         <f>VLOOKUP(C74,'Formato descripción HU'!B29:O29,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="E79" s="60"/>
+      <c r="E79" s="54"/>
       <c r="F79" s="17"/>
       <c r="G79" s="41" t="s">
         <v>74</v>
@@ -9559,8 +9559,8 @@
         <f>VLOOKUP(C74,'Formato descripción HU'!B29:O29,4,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I79" s="59"/>
-      <c r="J79" s="60"/>
+      <c r="I79" s="69"/>
+      <c r="J79" s="54"/>
       <c r="K79" s="17"/>
       <c r="L79" s="41" t="s">
         <v>75</v>
@@ -9576,13 +9576,13 @@
     <row r="80" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="31"/>
       <c r="C80" s="42"/>
-      <c r="D80" s="61"/>
-      <c r="E80" s="62"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="65"/>
       <c r="F80" s="17"/>
       <c r="G80" s="42"/>
-      <c r="H80" s="61"/>
+      <c r="H80" s="64"/>
       <c r="I80" s="40"/>
-      <c r="J80" s="62"/>
+      <c r="J80" s="65"/>
       <c r="K80" s="17"/>
       <c r="L80" s="42"/>
       <c r="M80" s="47"/>
@@ -9593,13 +9593,13 @@
     <row r="81" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="31"/>
       <c r="C81" s="43"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="65"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="56"/>
       <c r="F81" s="17"/>
       <c r="G81" s="43"/>
-      <c r="H81" s="63"/>
-      <c r="I81" s="64"/>
-      <c r="J81" s="65"/>
+      <c r="H81" s="55"/>
+      <c r="I81" s="70"/>
+      <c r="J81" s="56"/>
       <c r="K81" s="17"/>
       <c r="L81" s="43"/>
       <c r="M81" s="50"/>
@@ -9626,41 +9626,41 @@
     </row>
     <row r="83" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="31"/>
-      <c r="C83" s="67" t="s">
+      <c r="C83" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="D83" s="60"/>
-      <c r="E83" s="53" t="e">
+      <c r="D83" s="54"/>
+      <c r="E83" s="57" t="e">
         <f>VLOOKUP('Historia de Usuario'!C74,'Formato descripción HU'!B29:O29,14,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F83" s="54"/>
-      <c r="G83" s="54"/>
-      <c r="H83" s="54"/>
-      <c r="I83" s="54"/>
-      <c r="J83" s="54"/>
-      <c r="K83" s="54"/>
-      <c r="L83" s="54"/>
-      <c r="M83" s="54"/>
-      <c r="N83" s="54"/>
-      <c r="O83" s="55"/>
+      <c r="F83" s="58"/>
+      <c r="G83" s="58"/>
+      <c r="H83" s="58"/>
+      <c r="I83" s="58"/>
+      <c r="J83" s="58"/>
+      <c r="K83" s="58"/>
+      <c r="L83" s="58"/>
+      <c r="M83" s="58"/>
+      <c r="N83" s="58"/>
+      <c r="O83" s="59"/>
       <c r="P83" s="32"/>
     </row>
     <row r="84" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="31"/>
-      <c r="C84" s="63"/>
-      <c r="D84" s="65"/>
-      <c r="E84" s="56"/>
-      <c r="F84" s="57"/>
-      <c r="G84" s="57"/>
-      <c r="H84" s="57"/>
-      <c r="I84" s="57"/>
-      <c r="J84" s="57"/>
-      <c r="K84" s="57"/>
-      <c r="L84" s="57"/>
-      <c r="M84" s="57"/>
-      <c r="N84" s="57"/>
-      <c r="O84" s="58"/>
+      <c r="C84" s="55"/>
+      <c r="D84" s="56"/>
+      <c r="E84" s="60"/>
+      <c r="F84" s="61"/>
+      <c r="G84" s="61"/>
+      <c r="H84" s="61"/>
+      <c r="I84" s="61"/>
+      <c r="J84" s="61"/>
+      <c r="K84" s="61"/>
+      <c r="L84" s="61"/>
+      <c r="M84" s="61"/>
+      <c r="N84" s="61"/>
+      <c r="O84" s="62"/>
       <c r="P84" s="32"/>
     </row>
     <row r="85" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9682,10 +9682,10 @@
     </row>
     <row r="86" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="31"/>
-      <c r="C86" s="66" t="s">
+      <c r="C86" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="D86" s="60"/>
+      <c r="D86" s="54"/>
       <c r="E86" s="44" t="e">
         <f>VLOOKUP(C74,'Formato descripción HU'!B29:O29,12,0)</f>
         <v>#N/A</v>
@@ -9694,10 +9694,10 @@
       <c r="G86" s="45"/>
       <c r="H86" s="46"/>
       <c r="I86" s="17"/>
-      <c r="J86" s="66" t="s">
+      <c r="J86" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="K86" s="60"/>
+      <c r="K86" s="54"/>
       <c r="L86" s="44" t="e">
         <f>VLOOKUP(C74,'Formato descripción HU'!B29:O29,13,0)</f>
         <v>#N/A</v>
@@ -9709,15 +9709,15 @@
     </row>
     <row r="87" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="31"/>
-      <c r="C87" s="61"/>
-      <c r="D87" s="62"/>
+      <c r="C87" s="64"/>
+      <c r="D87" s="65"/>
       <c r="E87" s="47"/>
       <c r="F87" s="48"/>
       <c r="G87" s="48"/>
       <c r="H87" s="49"/>
       <c r="I87" s="17"/>
-      <c r="J87" s="61"/>
-      <c r="K87" s="62"/>
+      <c r="J87" s="64"/>
+      <c r="K87" s="65"/>
       <c r="L87" s="47"/>
       <c r="M87" s="48"/>
       <c r="N87" s="48"/>
@@ -9726,15 +9726,15 @@
     </row>
     <row r="88" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="31"/>
-      <c r="C88" s="63"/>
-      <c r="D88" s="65"/>
+      <c r="C88" s="55"/>
+      <c r="D88" s="56"/>
       <c r="E88" s="50"/>
       <c r="F88" s="51"/>
       <c r="G88" s="51"/>
       <c r="H88" s="52"/>
       <c r="I88" s="17"/>
-      <c r="J88" s="63"/>
-      <c r="K88" s="65"/>
+      <c r="J88" s="55"/>
+      <c r="K88" s="56"/>
       <c r="L88" s="50"/>
       <c r="M88" s="51"/>
       <c r="N88" s="51"/>
@@ -9833,15 +9833,15 @@
         <v>1</v>
       </c>
       <c r="D95" s="16"/>
-      <c r="E95" s="68" t="s">
+      <c r="E95" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F95" s="69"/>
+      <c r="F95" s="67"/>
       <c r="G95" s="16"/>
-      <c r="H95" s="68" t="s">
+      <c r="H95" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I95" s="69"/>
+      <c r="I95" s="67"/>
       <c r="J95" s="17"/>
       <c r="K95" s="17"/>
       <c r="L95" s="17"/>
@@ -9856,11 +9856,11 @@
         <v>29</v>
       </c>
       <c r="D96" s="19"/>
-      <c r="E96" s="70" t="e">
+      <c r="E96" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C96,'Formato descripción HU'!B51:O51,5,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F96" s="69"/>
+      <c r="F96" s="67"/>
       <c r="G96" s="20"/>
       <c r="H96" s="73" t="e">
         <f>VLOOKUP('Historia de Usuario'!C96,'Formato descripción HU'!B51:O51,11,0)</f>
@@ -9898,15 +9898,15 @@
         <v>71</v>
       </c>
       <c r="D98" s="19"/>
-      <c r="E98" s="68" t="s">
+      <c r="E98" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="F98" s="69"/>
+      <c r="F98" s="67"/>
       <c r="G98" s="20"/>
-      <c r="H98" s="68" t="s">
+      <c r="H98" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="I98" s="69"/>
+      <c r="I98" s="67"/>
       <c r="J98" s="20"/>
       <c r="K98" s="21"/>
       <c r="L98" s="21"/>
@@ -9922,17 +9922,17 @@
         <v>#N/A</v>
       </c>
       <c r="D99" s="19"/>
-      <c r="E99" s="70" t="e">
+      <c r="E99" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C96,'Formato descripción HU'!B51:O51,10,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F99" s="69"/>
+      <c r="F99" s="67"/>
       <c r="G99" s="20"/>
-      <c r="H99" s="70" t="e">
+      <c r="H99" s="68" t="e">
         <f>VLOOKUP('Historia de Usuario'!C96,'Formato descripción HU'!B51:O51,7,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I99" s="69"/>
+      <c r="I99" s="67"/>
       <c r="J99" s="20"/>
       <c r="K99" s="21"/>
       <c r="L99" s="21"/>
@@ -9967,7 +9967,7 @@
         <f>VLOOKUP(C96,'Formato descripción HU'!B51:O51,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="E101" s="60"/>
+      <c r="E101" s="54"/>
       <c r="F101" s="17"/>
       <c r="G101" s="41" t="s">
         <v>74</v>
@@ -9976,8 +9976,8 @@
         <f>VLOOKUP(C96,'Formato descripción HU'!B51:O51,4,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I101" s="59"/>
-      <c r="J101" s="60"/>
+      <c r="I101" s="69"/>
+      <c r="J101" s="54"/>
       <c r="K101" s="17"/>
       <c r="L101" s="41" t="s">
         <v>75</v>
@@ -9993,13 +9993,13 @@
     <row r="102" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="31"/>
       <c r="C102" s="42"/>
-      <c r="D102" s="61"/>
-      <c r="E102" s="62"/>
+      <c r="D102" s="64"/>
+      <c r="E102" s="65"/>
       <c r="F102" s="17"/>
       <c r="G102" s="42"/>
-      <c r="H102" s="61"/>
+      <c r="H102" s="64"/>
       <c r="I102" s="40"/>
-      <c r="J102" s="62"/>
+      <c r="J102" s="65"/>
       <c r="K102" s="17"/>
       <c r="L102" s="42"/>
       <c r="M102" s="47"/>
@@ -10010,13 +10010,13 @@
     <row r="103" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="31"/>
       <c r="C103" s="43"/>
-      <c r="D103" s="63"/>
-      <c r="E103" s="65"/>
+      <c r="D103" s="55"/>
+      <c r="E103" s="56"/>
       <c r="F103" s="17"/>
       <c r="G103" s="43"/>
-      <c r="H103" s="63"/>
-      <c r="I103" s="64"/>
-      <c r="J103" s="65"/>
+      <c r="H103" s="55"/>
+      <c r="I103" s="70"/>
+      <c r="J103" s="56"/>
       <c r="K103" s="17"/>
       <c r="L103" s="43"/>
       <c r="M103" s="50"/>
@@ -10043,41 +10043,41 @@
     </row>
     <row r="105" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="31"/>
-      <c r="C105" s="67" t="s">
+      <c r="C105" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="D105" s="60"/>
-      <c r="E105" s="53" t="e">
+      <c r="D105" s="54"/>
+      <c r="E105" s="57" t="e">
         <f>VLOOKUP('Historia de Usuario'!C96,'Formato descripción HU'!B51:O51,14,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F105" s="54"/>
-      <c r="G105" s="54"/>
-      <c r="H105" s="54"/>
-      <c r="I105" s="54"/>
-      <c r="J105" s="54"/>
-      <c r="K105" s="54"/>
-      <c r="L105" s="54"/>
-      <c r="M105" s="54"/>
-      <c r="N105" s="54"/>
-      <c r="O105" s="55"/>
+      <c r="F105" s="58"/>
+      <c r="G105" s="58"/>
+      <c r="H105" s="58"/>
+      <c r="I105" s="58"/>
+      <c r="J105" s="58"/>
+      <c r="K105" s="58"/>
+      <c r="L105" s="58"/>
+      <c r="M105" s="58"/>
+      <c r="N105" s="58"/>
+      <c r="O105" s="59"/>
       <c r="P105" s="32"/>
     </row>
     <row r="106" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="31"/>
-      <c r="C106" s="63"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="56"/>
-      <c r="F106" s="57"/>
-      <c r="G106" s="57"/>
-      <c r="H106" s="57"/>
-      <c r="I106" s="57"/>
-      <c r="J106" s="57"/>
-      <c r="K106" s="57"/>
-      <c r="L106" s="57"/>
-      <c r="M106" s="57"/>
-      <c r="N106" s="57"/>
-      <c r="O106" s="58"/>
+      <c r="C106" s="55"/>
+      <c r="D106" s="56"/>
+      <c r="E106" s="60"/>
+      <c r="F106" s="61"/>
+      <c r="G106" s="61"/>
+      <c r="H106" s="61"/>
+      <c r="I106" s="61"/>
+      <c r="J106" s="61"/>
+      <c r="K106" s="61"/>
+      <c r="L106" s="61"/>
+      <c r="M106" s="61"/>
+      <c r="N106" s="61"/>
+      <c r="O106" s="62"/>
       <c r="P106" s="32"/>
     </row>
     <row r="107" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10099,10 +10099,10 @@
     </row>
     <row r="108" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="31"/>
-      <c r="C108" s="66" t="s">
+      <c r="C108" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="D108" s="60"/>
+      <c r="D108" s="54"/>
       <c r="E108" s="44" t="e">
         <f>VLOOKUP(C96,'Formato descripción HU'!B51:O51,12,0)</f>
         <v>#N/A</v>
@@ -10111,10 +10111,10 @@
       <c r="G108" s="45"/>
       <c r="H108" s="46"/>
       <c r="I108" s="17"/>
-      <c r="J108" s="66" t="s">
+      <c r="J108" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="K108" s="60"/>
+      <c r="K108" s="54"/>
       <c r="L108" s="44" t="e">
         <f>VLOOKUP(C96,'Formato descripción HU'!B51:O51,13,0)</f>
         <v>#N/A</v>
@@ -10126,15 +10126,15 @@
     </row>
     <row r="109" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="31"/>
-      <c r="C109" s="61"/>
-      <c r="D109" s="62"/>
+      <c r="C109" s="64"/>
+      <c r="D109" s="65"/>
       <c r="E109" s="47"/>
       <c r="F109" s="48"/>
       <c r="G109" s="48"/>
       <c r="H109" s="49"/>
       <c r="I109" s="17"/>
-      <c r="J109" s="61"/>
-      <c r="K109" s="62"/>
+      <c r="J109" s="64"/>
+      <c r="K109" s="65"/>
       <c r="L109" s="47"/>
       <c r="M109" s="48"/>
       <c r="N109" s="48"/>
@@ -10143,15 +10143,15 @@
     </row>
     <row r="110" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="31"/>
-      <c r="C110" s="63"/>
-      <c r="D110" s="65"/>
+      <c r="C110" s="55"/>
+      <c r="D110" s="56"/>
       <c r="E110" s="50"/>
       <c r="F110" s="51"/>
       <c r="G110" s="51"/>
       <c r="H110" s="52"/>
       <c r="I110" s="17"/>
-      <c r="J110" s="63"/>
-      <c r="K110" s="65"/>
+      <c r="J110" s="55"/>
+      <c r="K110" s="56"/>
       <c r="L110" s="50"/>
       <c r="M110" s="51"/>
       <c r="N110" s="51"/>
@@ -11103,39 +11103,53 @@
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="L101:L103"/>
-    <mergeCell ref="M101:O103"/>
-    <mergeCell ref="C105:D106"/>
-    <mergeCell ref="E105:O106"/>
-    <mergeCell ref="C108:D110"/>
-    <mergeCell ref="E108:H110"/>
-    <mergeCell ref="J108:K110"/>
-    <mergeCell ref="L108:O110"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="C101:C103"/>
-    <mergeCell ref="D101:E103"/>
-    <mergeCell ref="G101:G103"/>
-    <mergeCell ref="H101:J103"/>
-    <mergeCell ref="B92:P92"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="M79:O81"/>
-    <mergeCell ref="C83:D84"/>
-    <mergeCell ref="E83:O84"/>
-    <mergeCell ref="C86:D88"/>
-    <mergeCell ref="E86:H88"/>
-    <mergeCell ref="J86:K88"/>
-    <mergeCell ref="L86:O88"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="D79:E81"/>
-    <mergeCell ref="G79:G81"/>
-    <mergeCell ref="H79:J81"/>
-    <mergeCell ref="L79:L81"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="M57:O59"/>
+    <mergeCell ref="E61:O62"/>
+    <mergeCell ref="E64:H66"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="H36:J38"/>
+    <mergeCell ref="C43:D45"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="J64:K66"/>
+    <mergeCell ref="L64:O66"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="D57:E59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="H57:J59"/>
+    <mergeCell ref="C64:D66"/>
+    <mergeCell ref="C61:D62"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B48:P48"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="C22:D24"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="E22:H24"/>
+    <mergeCell ref="J22:K24"/>
+    <mergeCell ref="L22:O24"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D15:E17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="L36:L38"/>
+    <mergeCell ref="M36:O38"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E40:O41"/>
     <mergeCell ref="E74:F74"/>
     <mergeCell ref="H74:I74"/>
     <mergeCell ref="E76:F76"/>
@@ -11160,53 +11174,39 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="D36:E38"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="L36:L38"/>
-    <mergeCell ref="M36:O38"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="E19:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E40:O41"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="C22:D24"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="E22:H24"/>
-    <mergeCell ref="J22:K24"/>
-    <mergeCell ref="L22:O24"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D15:E17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="M57:O59"/>
-    <mergeCell ref="E61:O62"/>
-    <mergeCell ref="E64:H66"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="H36:J38"/>
-    <mergeCell ref="C43:D45"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="J64:K66"/>
-    <mergeCell ref="L64:O66"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="D57:E59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="H57:J59"/>
-    <mergeCell ref="C64:D66"/>
-    <mergeCell ref="C61:D62"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B48:P48"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="B92:P92"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="M79:O81"/>
+    <mergeCell ref="C83:D84"/>
+    <mergeCell ref="E83:O84"/>
+    <mergeCell ref="C86:D88"/>
+    <mergeCell ref="E86:H88"/>
+    <mergeCell ref="J86:K88"/>
+    <mergeCell ref="L86:O88"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="D79:E81"/>
+    <mergeCell ref="G79:G81"/>
+    <mergeCell ref="H79:J81"/>
+    <mergeCell ref="L79:L81"/>
+    <mergeCell ref="L101:L103"/>
+    <mergeCell ref="M101:O103"/>
+    <mergeCell ref="C105:D106"/>
+    <mergeCell ref="E105:O106"/>
+    <mergeCell ref="C108:D110"/>
+    <mergeCell ref="E108:H110"/>
+    <mergeCell ref="J108:K110"/>
+    <mergeCell ref="L108:O110"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="D101:E103"/>
+    <mergeCell ref="G101:G103"/>
+    <mergeCell ref="H101:J103"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">

</xml_diff>